<commit_message>
time step to cost stores weekly
</commit_message>
<xml_diff>
--- a/data/GeneralInputCosts.xlsx
+++ b/data/GeneralInputCosts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlopalazzi/Programming/shipping_sprint/lcoa_model/lcoa-opt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9085FF3-D11E-214B-97F5-4B90197AE19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB60517A-B8D4-3645-BE0D-4F9413939C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16120" yWindow="-18880" windowWidth="16300" windowHeight="17500" activeTab="2" xr2:uid="{A11FE8FD-DB30-4178-A38C-42FEF5E50A0D}"/>
+    <workbookView xWindow="1040" yWindow="500" windowWidth="27760" windowHeight="17500" activeTab="2" xr2:uid="{A11FE8FD-DB30-4178-A38C-42FEF5E50A0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Trajectories" sheetId="2" r:id="rId1"/>
@@ -18,28 +18,6 @@
     <sheet name="Costs" sheetId="4" r:id="rId3"/>
     <sheet name="Efficiencies" sheetId="5" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Cost Trajectories'!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Cost Trajectories'!$A$2</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Cost Trajectories'!$A$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Cost Trajectories'!$A$2</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Cost Trajectories'!$A$3</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Cost Trajectories'!$A$4</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Cost Trajectories'!$A$5</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Cost Trajectories'!$B$1:$AG$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Cost Trajectories'!$B$2:$AG$2</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Cost Trajectories'!$B$3:$AG$3</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'Cost Trajectories'!$B$4:$AG$4</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'Cost Trajectories'!$B$5:$AG$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Cost Trajectories'!$A$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Cost Trajectories'!$A$4</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Cost Trajectories'!$A$5</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Cost Trajectories'!$B$1:$AG$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Cost Trajectories'!$B$2:$AG$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Cost Trajectories'!$B$3:$AG$3</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Cost Trajectories'!$B$4:$AG$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Cost Trajectories'!$B$5:$AG$5</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -796,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D610997-6B81-4F41-B7A2-83912DF5638D}">
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AG5"/>
     </sheetView>
   </sheetViews>
@@ -1573,7 +1551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34743C51-4234-4A9B-98D5-1B0DA6F3EF1C}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13:G17"/>
     </sheetView>
   </sheetViews>
@@ -2457,7 +2435,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>